<commit_message>
0.0.18: adapt package search to packageSuffix and overridePackage option.
</commit_message>
<xml_diff>
--- a/meta/program/BlancoValueObjectKtConstants.xlsx
+++ b/meta/program/BlancoValueObjectKtConstants.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoValueObjectKt/meta/program/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E1AD5AA-D55F-4149-A385-A3022CD34972}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4B13FC9-ECB7-E74C-9C75-83496D761B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1580" yWindow="1300" windowWidth="20040" windowHeight="15020" tabRatio="575" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -224,15 +224,15 @@
     <phoneticPr fontId="4"/>
   </si>
   <si>
-    <t>"0.0.1"</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
     <t>"/valueobjectkt"</t>
     <phoneticPr fontId="4"/>
   </si>
   <si>
     <t>"main/kotlin"</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>"0.0.18"</t>
     <phoneticPr fontId="4"/>
   </si>
 </sst>
@@ -1076,7 +1076,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -1120,7 +1120,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -1148,7 +1148,7 @@
   <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1387,7 +1387,7 @@
         <v>22</v>
       </c>
       <c r="D22" s="26" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E22" s="26" t="s">
         <v>27</v>
@@ -1407,7 +1407,7 @@
         <v>22</v>
       </c>
       <c r="D23" s="26" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E23" s="26" t="s">
         <v>29</v>
@@ -1507,7 +1507,7 @@
         <v>33</v>
       </c>
       <c r="D28" s="26" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E28" s="26" t="s">
         <v>41</v>

</xml_diff>

<commit_message>
0.0.20: Enable searchTmpdir option to search package by SimpleClass name.
</commit_message>
<xml_diff>
--- a/meta/program/BlancoValueObjectKtConstants.xlsx
+++ b/meta/program/BlancoValueObjectKtConstants.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoValueObjectKt/meta/program/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F60889EC-D0B4-5843-9A0A-FE2078A5D2D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABF16586-ACD1-D84F-B252-F2DBF3DAC33C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1580" yWindow="1300" windowWidth="20040" windowHeight="15020" tabRatio="575" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -232,7 +232,7 @@
     <phoneticPr fontId="4"/>
   </si>
   <si>
-    <t>"0.0.19"</t>
+    <t>"0.0.20"</t>
     <phoneticPr fontId="4"/>
   </si>
 </sst>
@@ -1076,7 +1076,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -1120,7 +1120,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -1148,7 +1148,7 @@
   <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>

</xml_diff>

<commit_message>
0.0.22: field annotation should be lead by field keyword on kotlin.
</commit_message>
<xml_diff>
--- a/meta/program/BlancoValueObjectKtConstants.xlsx
+++ b/meta/program/BlancoValueObjectKtConstants.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoValueObjectKt/meta/program/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDBE353B-48E3-8F45-94C6-ADEA1C0C24C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F3C1E8A-DB2C-7346-BA26-F1A042EB683A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1580" yWindow="1300" windowWidth="20040" windowHeight="15020" tabRatio="575" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -232,7 +232,7 @@
     <phoneticPr fontId="4"/>
   </si>
   <si>
-    <t>"0.0.21"</t>
+    <t>"0.0.22"</t>
     <phoneticPr fontId="4"/>
   </si>
 </sst>
@@ -1076,7 +1076,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -1120,7 +1120,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -1148,7 +1148,7 @@
   <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>

</xml_diff>

<commit_message>
3.0.3: Support inheritance with constructor arguments. * Specify open and constArg flag in super class. * Specify override and constArg flag in sub class.
</commit_message>
<xml_diff>
--- a/meta/program/BlancoValueObjectKtConstants.xlsx
+++ b/meta/program/BlancoValueObjectKtConstants.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoValueObjectKt/meta/program/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60F3E2A6-0F04-9E4F-83D2-73CD1BADD0D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4826894A-F8FC-1C4D-957E-01FAFA534143}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1580" yWindow="1300" windowWidth="20040" windowHeight="15020" tabRatio="575" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -232,7 +232,7 @@
     <phoneticPr fontId="4"/>
   </si>
   <si>
-    <t>"0.1.0"</t>
+    <t>"3.0.3"</t>
     <phoneticPr fontId="4"/>
   </si>
 </sst>
@@ -578,29 +578,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -661,7 +660,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
@@ -670,10 +669,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
@@ -682,7 +681,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1076,7 +1075,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -1120,7 +1119,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -1230,43 +1229,43 @@
         <v>9</v>
       </c>
       <c r="D9"/>
-      <c r="E9" s="15"/>
+      <c r="E9"/>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="17"/>
-      <c r="C10" s="18" t="s">
+      <c r="B10" s="16"/>
+      <c r="C10" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
+      <c r="D10"/>
+      <c r="E10"/>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="16" t="s">
+      <c r="A11" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="17"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15"/>
+      <c r="B11" s="16"/>
+      <c r="C11" s="17"/>
+      <c r="D11"/>
+      <c r="E11"/>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="16" t="s">
+      <c r="A12" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="17"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="15"/>
+      <c r="B12" s="16"/>
+      <c r="C12" s="17"/>
+      <c r="D12"/>
+      <c r="E12"/>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="15"/>
-      <c r="B13" s="15"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="15"/>
+      <c r="A13"/>
+      <c r="B13"/>
+      <c r="C13"/>
+      <c r="D13"/>
+      <c r="E13"/>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="4" t="s">
@@ -1278,13 +1277,13 @@
       <c r="E14" s="6"/>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="16" t="s">
+      <c r="A15" s="15" t="s">
         <v>15</v>
       </c>
       <c r="B15" s="7"/>
-      <c r="C15" s="19"/>
-      <c r="D15" s="20"/>
-      <c r="E15" s="21"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="20"/>
     </row>
     <row r="16" spans="1:6">
       <c r="A16"/>
@@ -1298,251 +1297,251 @@
       <c r="A17" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="17"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
+      <c r="B17" s="16"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="16"/>
       <c r="F17" s="7"/>
       <c r="G17"/>
       <c r="H17"/>
     </row>
     <row r="18" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A18" s="44" t="s">
+      <c r="A18" s="43" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="44" t="s">
+      <c r="B18" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="45" t="s">
+      <c r="C18" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="D18" s="45" t="s">
+      <c r="D18" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="E18" s="45" t="s">
+      <c r="E18" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="F18" s="22"/>
+      <c r="F18" s="21"/>
       <c r="G18"/>
       <c r="H18"/>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="44"/>
-      <c r="B19" s="44"/>
-      <c r="C19" s="45"/>
-      <c r="D19" s="45"/>
-      <c r="E19" s="45"/>
-      <c r="F19" s="23"/>
+      <c r="A19" s="43"/>
+      <c r="B19" s="43"/>
+      <c r="C19" s="44"/>
+      <c r="D19" s="44"/>
+      <c r="E19" s="44"/>
+      <c r="F19" s="22"/>
       <c r="G19"/>
       <c r="H19"/>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="24">
+      <c r="A20" s="23">
         <v>1</v>
       </c>
-      <c r="B20" s="25" t="s">
+      <c r="B20" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="26" t="s">
+      <c r="C20" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="D20" s="26" t="s">
+      <c r="D20" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="E20" s="27" t="s">
+      <c r="E20" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="F20" s="28"/>
+      <c r="F20" s="27"/>
       <c r="G20"/>
       <c r="H20"/>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" s="24">
+      <c r="A21" s="23">
         <v>2</v>
       </c>
-      <c r="B21" s="25" t="s">
+      <c r="B21" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="C21" s="26" t="s">
+      <c r="C21" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="D21" s="26" t="s">
+      <c r="D21" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="E21" s="29" t="s">
+      <c r="E21" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="F21" s="30"/>
+      <c r="F21" s="29"/>
       <c r="G21"/>
       <c r="H21"/>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" s="24">
+      <c r="A22" s="23">
         <v>3</v>
       </c>
-      <c r="B22" s="25" t="s">
+      <c r="B22" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="C22" s="26" t="s">
+      <c r="C22" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="D22" s="26" t="s">
+      <c r="D22" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="E22" s="26" t="s">
+      <c r="E22" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="F22" s="30"/>
+      <c r="F22" s="29"/>
       <c r="G22"/>
       <c r="H22"/>
     </row>
     <row r="23" spans="1:8">
-      <c r="A23" s="24">
+      <c r="A23" s="23">
         <v>4</v>
       </c>
-      <c r="B23" s="25" t="s">
+      <c r="B23" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="C23" s="26" t="s">
+      <c r="C23" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="D23" s="26" t="s">
+      <c r="D23" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="E23" s="26" t="s">
+      <c r="E23" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="F23" s="30"/>
+      <c r="F23" s="29"/>
       <c r="G23"/>
       <c r="H23"/>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" s="24">
+      <c r="A24" s="23">
         <v>5</v>
       </c>
-      <c r="B24" s="25" t="s">
+      <c r="B24" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="C24" s="26" t="s">
+      <c r="C24" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="D24" s="26" t="s">
+      <c r="D24" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="E24" s="26" t="s">
+      <c r="E24" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="F24" s="30"/>
+      <c r="F24" s="29"/>
       <c r="G24"/>
       <c r="H24"/>
     </row>
     <row r="25" spans="1:8">
-      <c r="A25" s="24">
+      <c r="A25" s="23">
         <v>6</v>
       </c>
-      <c r="B25" s="25" t="s">
+      <c r="B25" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="C25" s="26" t="s">
+      <c r="C25" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="D25" s="26" t="s">
+      <c r="D25" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="E25" s="26" t="s">
+      <c r="E25" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="F25" s="30"/>
+      <c r="F25" s="29"/>
       <c r="G25"/>
       <c r="H25"/>
     </row>
     <row r="26" spans="1:8">
-      <c r="A26" s="24">
+      <c r="A26" s="23">
         <v>7</v>
       </c>
-      <c r="B26" s="25" t="s">
+      <c r="B26" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="C26" s="26" t="s">
+      <c r="C26" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="D26" s="26" t="s">
+      <c r="D26" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="E26" s="26" t="s">
+      <c r="E26" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="F26" s="30"/>
+      <c r="F26" s="29"/>
       <c r="G26"/>
       <c r="H26"/>
     </row>
     <row r="27" spans="1:8">
-      <c r="A27" s="24">
+      <c r="A27" s="23">
         <v>8</v>
       </c>
-      <c r="B27" s="25" t="s">
+      <c r="B27" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="C27" s="26" t="s">
+      <c r="C27" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="D27" s="26" t="s">
+      <c r="D27" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="E27" s="26" t="s">
+      <c r="E27" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="F27" s="30"/>
+      <c r="F27" s="29"/>
       <c r="G27"/>
       <c r="H27"/>
     </row>
     <row r="28" spans="1:8">
-      <c r="A28" s="24">
+      <c r="A28" s="23">
         <v>8</v>
       </c>
-      <c r="B28" s="25" t="s">
+      <c r="B28" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="C28" s="26" t="s">
+      <c r="C28" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="D28" s="26" t="s">
+      <c r="D28" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="E28" s="26" t="s">
+      <c r="E28" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="F28" s="33"/>
+      <c r="F28" s="32"/>
       <c r="G28"/>
       <c r="H28"/>
     </row>
     <row r="29" spans="1:8">
-      <c r="A29" s="31"/>
-      <c r="B29" s="25"/>
-      <c r="C29" s="32"/>
-      <c r="D29" s="32"/>
-      <c r="E29" s="32"/>
-      <c r="F29" s="33"/>
+      <c r="A29" s="30"/>
+      <c r="B29" s="24"/>
+      <c r="C29" s="31"/>
+      <c r="D29" s="31"/>
+      <c r="E29" s="31"/>
+      <c r="F29" s="32"/>
       <c r="G29"/>
       <c r="H29"/>
     </row>
     <row r="30" spans="1:8">
-      <c r="A30" s="31"/>
-      <c r="B30" s="25"/>
-      <c r="C30" s="32"/>
-      <c r="D30" s="32"/>
-      <c r="E30" s="32"/>
-      <c r="F30" s="33"/>
+      <c r="A30" s="30"/>
+      <c r="B30" s="24"/>
+      <c r="C30" s="31"/>
+      <c r="D30" s="31"/>
+      <c r="E30" s="31"/>
+      <c r="F30" s="32"/>
       <c r="G30"/>
       <c r="H30"/>
     </row>
     <row r="31" spans="1:8">
-      <c r="A31" s="34"/>
-      <c r="B31" s="35"/>
-      <c r="C31" s="36"/>
-      <c r="D31" s="36"/>
-      <c r="E31" s="36"/>
-      <c r="F31" s="37"/>
+      <c r="A31" s="33"/>
+      <c r="B31" s="34"/>
+      <c r="C31" s="35"/>
+      <c r="D31" s="35"/>
+      <c r="E31" s="35"/>
+      <c r="F31" s="36"/>
       <c r="G31"/>
       <c r="H31"/>
     </row>
@@ -1621,34 +1620,34 @@
       </c>
     </row>
     <row r="3" spans="1:10">
-      <c r="B3" s="38" t="s">
+      <c r="B3" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="38" t="s">
+      <c r="D3" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="38" t="s">
+      <c r="F3" s="37" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:10">
-      <c r="B4" s="39"/>
-      <c r="D4" s="40"/>
-      <c r="F4" s="40"/>
+      <c r="B4" s="38"/>
+      <c r="D4" s="39"/>
+      <c r="F4" s="39"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="B5" s="41" t="s">
+      <c r="B5" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="42" t="s">
+      <c r="D5" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="F5" s="42" t="s">
+      <c r="F5" s="41" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="B6" s="43"/>
+      <c r="B6" s="42"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>

</xml_diff>

<commit_message>
3.0.5: Implement serdeable option to supply @Serdeable annotaion generally.
</commit_message>
<xml_diff>
--- a/meta/program/BlancoValueObjectKtConstants.xlsx
+++ b/meta/program/BlancoValueObjectKtConstants.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoValueObjectKt/meta/program/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4826894A-F8FC-1C4D-957E-01FAFA534143}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD331C9E-B556-2543-AE3E-D7D22400B3A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1580" yWindow="1300" windowWidth="20040" windowHeight="15020" tabRatio="575" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -232,7 +232,7 @@
     <phoneticPr fontId="4"/>
   </si>
   <si>
-    <t>"3.0.3"</t>
+    <t>"3.0.5"</t>
     <phoneticPr fontId="4"/>
   </si>
 </sst>
@@ -1075,7 +1075,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -1119,7 +1119,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">

</xml_diff>

<commit_message>
3.0.6: Support annotation for Enum class.
</commit_message>
<xml_diff>
--- a/meta/program/BlancoValueObjectKtConstants.xlsx
+++ b/meta/program/BlancoValueObjectKtConstants.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoValueObjectKt/meta/program/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD331C9E-B556-2543-AE3E-D7D22400B3A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E851D347-84E1-A941-BB5B-0CAC3D0D7D13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1580" yWindow="1300" windowWidth="20040" windowHeight="15020" tabRatio="575" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -232,7 +232,7 @@
     <phoneticPr fontId="4"/>
   </si>
   <si>
-    <t>"3.0.5"</t>
+    <t>"3.0.6"</t>
     <phoneticPr fontId="4"/>
   </si>
 </sst>
@@ -1075,7 +1075,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -1119,7 +1119,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">

</xml_diff>

<commit_message>
3.0.7: Implement ignoreUnknown option to add @JsonIgnoreProperties(ignoreUnknown = true) annotation.
</commit_message>
<xml_diff>
--- a/meta/program/BlancoValueObjectKtConstants.xlsx
+++ b/meta/program/BlancoValueObjectKtConstants.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoValueObjectKt/meta/program/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E851D347-84E1-A941-BB5B-0CAC3D0D7D13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{774488D2-C969-4E4F-A554-58107DF5A04B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1580" yWindow="1300" windowWidth="20040" windowHeight="15020" tabRatio="575" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -232,7 +232,7 @@
     <phoneticPr fontId="4"/>
   </si>
   <si>
-    <t>"3.0.6"</t>
+    <t>"3.0.7"</t>
     <phoneticPr fontId="4"/>
   </si>
 </sst>
@@ -1075,7 +1075,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -1119,7 +1119,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">

</xml_diff>

<commit_message>
3.0.8: Fix typo of option...
</commit_message>
<xml_diff>
--- a/meta/program/BlancoValueObjectKtConstants.xlsx
+++ b/meta/program/BlancoValueObjectKtConstants.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoValueObjectKt/meta/program/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{774488D2-C969-4E4F-A554-58107DF5A04B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA037243-6CC7-B146-AA3A-D5FFEE710547}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1580" yWindow="1300" windowWidth="20040" windowHeight="15020" tabRatio="575" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -232,7 +232,7 @@
     <phoneticPr fontId="4"/>
   </si>
   <si>
-    <t>"3.0.7"</t>
+    <t>"3.0.8"</t>
     <phoneticPr fontId="4"/>
   </si>
 </sst>
@@ -1075,7 +1075,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -1119,7 +1119,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">

</xml_diff>

<commit_message>
3.0.12: No @field:NotNull and @Nullable annotations are added if enum class.
</commit_message>
<xml_diff>
--- a/meta/program/BlancoValueObjectKtConstants.xlsx
+++ b/meta/program/BlancoValueObjectKtConstants.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoValueObjectKt/meta/program/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41470A90-ED05-2447-905B-04F2C5A74139}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F644EFFA-C2F2-EE4D-A477-A2CBFB09C62D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1580" yWindow="1300" windowWidth="20040" windowHeight="15020" tabRatio="575" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -232,7 +232,7 @@
     <phoneticPr fontId="4"/>
   </si>
   <si>
-    <t>"3.0.11"</t>
+    <t>"3.0.12"</t>
     <phoneticPr fontId="4"/>
   </si>
 </sst>
@@ -1075,7 +1075,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -1119,7 +1119,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -1147,7 +1147,7 @@
   <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>

</xml_diff>